<commit_message>
changes in linkelist datastrusture graph register testData.xlsx
</commit_message>
<xml_diff>
--- a/src/test/resources/excelTestData/testData.xlsx
+++ b/src/test/resources/excelTestData/testData.xlsx
@@ -1,16 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{6938C4EF-814D-4467-959D-87FEC8D00173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Register_invalid" sheetId="1" r:id="rId1"/>
     <sheet name="Register_valid" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:Q33"/>
 </workbook>
 </file>
 
@@ -92,8 +94,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,9 +148,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -186,7 +188,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -220,6 +222,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -254,9 +257,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -429,14 +433,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="48.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" customWidth="1"/>
@@ -444,7 +448,7 @@
     <col min="4" max="4" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -458,7 +462,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -472,7 +476,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -486,7 +490,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -500,7 +504,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -514,7 +518,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -528,7 +532,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -542,7 +546,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -556,7 +560,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -570,7 +574,7 @@
         <v>12345</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -584,7 +588,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -598,7 +602,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -614,14 +618,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="C4" r:id="rId2"/>
-    <hyperlink ref="C5" r:id="rId3"/>
-    <hyperlink ref="D5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B7" r:id="rId6"/>
-    <hyperlink ref="D6" r:id="rId7"/>
-    <hyperlink ref="C7" r:id="rId8"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="D6" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C7" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId9"/>
@@ -629,14 +633,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.85546875" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
@@ -644,7 +648,7 @@
     <col min="4" max="4" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -658,7 +662,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
commit feature files java page stepDef runner
</commit_message>
<xml_diff>
--- a/src/test/resources/excelTestData/testData.xlsx
+++ b/src/test/resources/excelTestData/testData.xlsx
@@ -3,16 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{6938C4EF-814D-4467-959D-87FEC8D00173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0EA17FB3-0DD6-4DF8-91C5-3D94A512243B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Register_invalid" sheetId="1" r:id="rId1"/>
     <sheet name="Register_valid" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:Q33"/>
+  <oleSize ref="A1:U7"/>
 </workbook>
 </file>
 
@@ -436,7 +436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A12" sqref="A12:D12"/>
     </sheetView>
   </sheetViews>
@@ -636,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
commit register page feature file stepDef
</commit_message>
<xml_diff>
--- a/src/test/resources/excelTestData/testData.xlsx
+++ b/src/test/resources/excelTestData/testData.xlsx
@@ -1,18 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0EA17FB3-0DD6-4DF8-91C5-3D94A512243B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Register_invalid" sheetId="1" r:id="rId1"/>
     <sheet name="Register_valid" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1:U7"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -46,12 +44,6 @@
     <t>hj7</t>
   </si>
   <si>
-    <t>mita@67</t>
-  </si>
-  <si>
-    <t>qwer1234</t>
-  </si>
-  <si>
     <t>ScenarioName</t>
   </si>
   <si>
@@ -89,13 +81,19 @@
   </si>
   <si>
     <t>validEntry</t>
+  </si>
+  <si>
+    <t>mita@671</t>
+  </si>
+  <si>
+    <t>qwerew123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,9 +146,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -188,7 +186,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -222,7 +220,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -257,10 +254,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -433,14 +429,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="48.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" customWidth="1"/>
@@ -448,9 +444,9 @@
     <col min="4" max="4" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -462,66 +458,66 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
@@ -532,9 +528,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
@@ -546,9 +542,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>7</v>
@@ -560,9 +556,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>4</v>
@@ -574,9 +570,9 @@
         <v>12345</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>4</v>
@@ -588,9 +584,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>4</v>
@@ -602,9 +598,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>4</v>
@@ -618,14 +614,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="D6" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="C7" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="C4" r:id="rId2"/>
+    <hyperlink ref="C5" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
+    <hyperlink ref="D6" r:id="rId7"/>
+    <hyperlink ref="C7" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId9"/>
@@ -633,14 +629,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.85546875" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
@@ -648,9 +644,9 @@
     <col min="4" max="4" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -662,18 +658,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>